<commit_message>
Added a few cocktails and more non alcohols
</commit_message>
<xml_diff>
--- a/alcohol.xlsx
+++ b/alcohol.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Michael\GitHub\Neuedelft\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{90AE81D2-0D35-40F0-BBC8-D72DFD5043F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC00E11E-36FA-4C8C-8D54-BE200F50643D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{075A0E28-8A96-48D6-B40D-E2D5A28BE5AD}"/>
+    <workbookView xWindow="7200" yWindow="30" windowWidth="21600" windowHeight="11295" xr2:uid="{075A0E28-8A96-48D6-B40D-E2D5A28BE5AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -329,6 +329,9 @@
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{734AC9A7-A10C-4054-ABE0-537832B7A544}" name="Table1" displayName="Table1" ref="A1:E64" totalsRowShown="0">
   <autoFilter ref="A1:E64" xr:uid="{734AC9A7-A10C-4054-ABE0-537832B7A544}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:E64">
+    <sortCondition ref="A1:A64"/>
+  </sortState>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{34AE03DE-8616-42CC-B469-73BA5FF24E2C}" name="id">
       <calculatedColumnFormula>LOWER(SUBSTITUTE(B2," ", "_"))</calculatedColumnFormula>
@@ -641,8 +644,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28EAB358-781B-44E4-9620-248CA4846061}">
   <dimension ref="A1:H64"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="S12" sqref="S12"/>
+    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
+      <selection activeCell="C61" sqref="C61"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -684,7 +687,7 @@
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="str">
-        <f t="shared" ref="A3:A64" si="0">LOWER(SUBSTITUTE(B3," ", "_"))</f>
+        <f>LOWER(SUBSTITUTE(B3," ", "_"))</f>
         <v>apfelkorn</v>
       </c>
       <c r="B3" t="s">
@@ -702,17 +705,17 @@
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="str">
-        <f t="shared" si="0"/>
-        <v>beerenburg</v>
+        <f>LOWER(SUBSTITUTE(B4," ", "_"))</f>
+        <v>bacardi_black</v>
       </c>
       <c r="B4" t="s">
-        <v>4</v>
+        <v>44</v>
       </c>
       <c r="C4">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="D4" s="1">
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
       <c r="E4">
         <v>40</v>
@@ -720,17 +723,17 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="str">
-        <f t="shared" si="0"/>
-        <v>brandewijn</v>
+        <f>LOWER(SUBSTITUTE(B5," ", "_"))</f>
+        <v>bacardi_blanca</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>45</v>
       </c>
       <c r="C5">
-        <v>35</v>
+        <v>37.5</v>
       </c>
       <c r="D5" s="1">
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
       <c r="E5">
         <v>40</v>
@@ -738,17 +741,17 @@
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="str">
-        <f t="shared" si="0"/>
-        <v>café_marakesh</v>
+        <f>LOWER(SUBSTITUTE(B6," ", "_"))</f>
+        <v>bacardi_lemon</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>46</v>
       </c>
       <c r="C6">
-        <v>23</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1">
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
       <c r="E6">
         <v>40</v>
@@ -756,17 +759,17 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="str">
-        <f t="shared" si="0"/>
-        <v>coebergh</v>
+        <f>LOWER(SUBSTITUTE(B7," ", "_"))</f>
+        <v>bacardi_razz</v>
       </c>
       <c r="B7" t="s">
-        <v>7</v>
+        <v>47</v>
       </c>
       <c r="C7">
-        <v>14.5</v>
+        <v>32</v>
       </c>
       <c r="D7" s="1">
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
       <c r="E7">
         <v>40</v>
@@ -774,17 +777,17 @@
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="str">
-        <f t="shared" si="0"/>
-        <v>dropshot</v>
+        <f>LOWER(SUBSTITUTE(B8," ", "_"))</f>
+        <v>baileys</v>
       </c>
       <c r="B8" t="s">
-        <v>8</v>
+        <v>20</v>
       </c>
       <c r="C8">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1">
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
       <c r="E8">
         <v>40</v>
@@ -792,14 +795,14 @@
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="str">
-        <f t="shared" si="0"/>
-        <v>fireball</v>
+        <f>LOWER(SUBSTITUTE(B9," ", "_"))</f>
+        <v>beerenburg</v>
       </c>
       <c r="B9" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C9">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="D9" s="1">
         <v>1.3</v>
@@ -810,14 +813,14 @@
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="str">
-        <f t="shared" si="0"/>
-        <v>ketel1</v>
+        <f>LOWER(SUBSTITUTE(B10," ", "_"))</f>
+        <v>bols_apple_sour</v>
       </c>
       <c r="B10" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="C10">
-        <v>35</v>
+        <v>17</v>
       </c>
       <c r="D10" s="1">
         <v>1.3</v>
@@ -828,14 +831,14 @@
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="str">
-        <f t="shared" si="0"/>
-        <v>malibu</v>
+        <f>LOWER(SUBSTITUTE(B11," ", "_"))</f>
+        <v>bols_blue_caracao</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>48</v>
       </c>
       <c r="C11">
-        <v>21</v>
+        <v>14.5</v>
       </c>
       <c r="D11" s="1">
         <v>1.3</v>
@@ -846,11 +849,11 @@
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="str">
-        <f t="shared" si="0"/>
-        <v>martini</v>
+        <f>LOWER(SUBSTITUTE(B12," ", "_"))</f>
+        <v>bols_crème_de_bananes</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>49</v>
       </c>
       <c r="C12">
         <v>15</v>
@@ -864,14 +867,14 @@
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="str">
-        <f t="shared" si="0"/>
-        <v>mede</v>
+        <f>LOWER(SUBSTITUTE(B13," ", "_"))</f>
+        <v>bols_crème_de_cassis</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>64</v>
       </c>
       <c r="C13">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="D13" s="1">
         <v>1.3</v>
@@ -882,14 +885,14 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="str">
-        <f t="shared" si="0"/>
-        <v>passao</v>
+        <f>LOWER(SUBSTITUTE(B14," ", "_"))</f>
+        <v>brandewijn</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>5</v>
       </c>
       <c r="C14">
-        <v>14.9</v>
+        <v>35</v>
       </c>
       <c r="D14" s="1">
         <v>1.3</v>
@@ -900,14 +903,14 @@
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="str">
-        <f t="shared" si="0"/>
-        <v>peach_tree</v>
+        <f>LOWER(SUBSTITUTE(B15," ", "_"))</f>
+        <v>café_marakesh</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>6</v>
       </c>
       <c r="C15">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="D15" s="1">
         <v>1.3</v>
@@ -918,14 +921,14 @@
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="str">
-        <f t="shared" si="0"/>
-        <v>peerkorn</v>
+        <f>LOWER(SUBSTITUTE(B16," ", "_"))</f>
+        <v>coebergh</v>
       </c>
       <c r="B16" t="s">
-        <v>62</v>
+        <v>7</v>
       </c>
       <c r="C16">
-        <v>15</v>
+        <v>14.5</v>
       </c>
       <c r="D16" s="1">
         <v>1.3</v>
@@ -936,17 +939,17 @@
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="str">
-        <f t="shared" si="0"/>
-        <v>pisang_ambon</v>
+        <f>LOWER(SUBSTITUTE(B17," ", "_"))</f>
+        <v>cognac</v>
       </c>
       <c r="B17" t="s">
-        <v>15</v>
+        <v>37</v>
       </c>
       <c r="C17">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="D17" s="1">
-        <v>1.3</v>
+        <v>3</v>
       </c>
       <c r="E17">
         <v>40</v>
@@ -954,17 +957,17 @@
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="str">
-        <f t="shared" si="0"/>
-        <v>safari</v>
+        <f>LOWER(SUBSTITUTE(B18," ", "_"))</f>
+        <v>cointreau</v>
       </c>
       <c r="B18" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="C18">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="D18" s="1">
-        <v>1.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E18">
         <v>40</v>
@@ -972,17 +975,17 @@
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="str">
-        <f t="shared" si="0"/>
-        <v>sippers_bitter</v>
+        <f>LOWER(SUBSTITUTE(B19," ", "_"))</f>
+        <v>disaronno</v>
       </c>
       <c r="B19" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="C19">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="D19" s="1">
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
       <c r="E19">
         <v>40</v>
@@ -990,11 +993,11 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="str">
-        <f t="shared" si="0"/>
-        <v>tia_maria</v>
+        <f>LOWER(SUBSTITUTE(B20," ", "_"))</f>
+        <v>dropshot</v>
       </c>
       <c r="B20" t="s">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="C20">
         <v>20</v>
@@ -1008,35 +1011,35 @@
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="str">
-        <f t="shared" si="0"/>
-        <v>hoppe_vieux</v>
+        <f>LOWER(SUBSTITUTE(B21," ", "_"))</f>
+        <v>estaminet</v>
       </c>
       <c r="B21" t="s">
-        <v>19</v>
+        <v>50</v>
       </c>
       <c r="C21">
-        <v>35</v>
+        <v>5.2</v>
       </c>
       <c r="D21" s="1">
-        <v>1.3</v>
+        <v>1.2</v>
       </c>
       <c r="E21">
-        <v>40</v>
+        <v>250</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="str">
-        <f t="shared" si="0"/>
-        <v>baileys</v>
+        <f>LOWER(SUBSTITUTE(B22," ", "_"))</f>
+        <v>fireball</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>9</v>
       </c>
       <c r="C22">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="D22" s="1">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="E22">
         <v>40</v>
@@ -1044,14 +1047,14 @@
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" t="str">
-        <f t="shared" si="0"/>
-        <v>disaronno</v>
+        <f>LOWER(SUBSTITUTE(B23," ", "_"))</f>
+        <v>frangelico</v>
       </c>
       <c r="B23" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C23">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="D23" s="1">
         <v>1.7</v>
@@ -1062,17 +1065,17 @@
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" t="str">
-        <f t="shared" si="0"/>
-        <v>frangelico</v>
+        <f>LOWER(SUBSTITUTE(B24," ", "_"))</f>
+        <v>friesengeist</v>
       </c>
       <c r="B24" t="s">
-        <v>22</v>
+        <v>32</v>
       </c>
       <c r="C24">
-        <v>20</v>
+        <v>56</v>
       </c>
       <c r="D24" s="1">
-        <v>1.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E24">
         <v>40</v>
@@ -1080,14 +1083,14 @@
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" t="str">
-        <f t="shared" si="0"/>
-        <v>gordon's_gin</v>
+        <f>LOWER(SUBSTITUTE(B25," ", "_"))</f>
+        <v>goldstrike</v>
       </c>
       <c r="B25" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C25">
-        <v>37.5</v>
+        <v>50</v>
       </c>
       <c r="D25" s="1">
         <v>1.7</v>
@@ -1098,14 +1101,14 @@
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" t="str">
-        <f t="shared" si="0"/>
-        <v>goldstrike</v>
+        <f>LOWER(SUBSTITUTE(B26," ", "_"))</f>
+        <v>gordon's_gin</v>
       </c>
       <c r="B26" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26">
-        <v>50</v>
+        <v>37.5</v>
       </c>
       <c r="D26" s="1">
         <v>1.7</v>
@@ -1116,17 +1119,17 @@
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" t="str">
-        <f t="shared" si="0"/>
-        <v>jägermeister</v>
+        <f>LOWER(SUBSTITUTE(B27," ", "_"))</f>
+        <v>grand_marnier</v>
       </c>
       <c r="B27" t="s">
-        <v>25</v>
+        <v>34</v>
       </c>
       <c r="C27">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="D27" s="1">
-        <v>1.7</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E27">
         <v>40</v>
@@ -1134,17 +1137,17 @@
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" t="str">
-        <f t="shared" si="0"/>
-        <v>jameson</v>
+        <f>LOWER(SUBSTITUTE(B28," ", "_"))</f>
+        <v>hagel_en_donder</v>
       </c>
       <c r="B28" t="s">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="C28">
-        <v>40</v>
+        <v>25</v>
       </c>
       <c r="D28" s="1">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="E28">
         <v>40</v>
@@ -1152,17 +1155,17 @@
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" t="str">
-        <f t="shared" si="0"/>
-        <v>juttertje</v>
+        <f>LOWER(SUBSTITUTE(B29," ", "_"))</f>
+        <v>hoppe_vieux</v>
       </c>
       <c r="B29" t="s">
-        <v>27</v>
+        <v>19</v>
       </c>
       <c r="C29">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="D29" s="1">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="E29">
         <v>40</v>
@@ -1170,14 +1173,14 @@
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" t="str">
-        <f t="shared" si="0"/>
-        <v>licor_43</v>
+        <f>LOWER(SUBSTITUTE(B30," ", "_"))</f>
+        <v>jägermeister</v>
       </c>
       <c r="B30" t="s">
-        <v>28</v>
+        <v>25</v>
       </c>
       <c r="C30">
-        <v>31</v>
+        <v>35</v>
       </c>
       <c r="D30" s="1">
         <v>1.7</v>
@@ -1188,11 +1191,11 @@
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" t="str">
-        <f t="shared" si="0"/>
-        <v>pernod</v>
+        <f>LOWER(SUBSTITUTE(B31," ", "_"))</f>
+        <v>jameson</v>
       </c>
       <c r="B31" t="s">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="C31">
         <v>40</v>
@@ -1206,14 +1209,14 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" t="str">
-        <f t="shared" si="0"/>
-        <v>sambuca</v>
+        <f>LOWER(SUBSTITUTE(B32," ", "_"))</f>
+        <v>juttertje</v>
       </c>
       <c r="B32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C32">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="D32" s="1">
         <v>1.7</v>
@@ -1224,17 +1227,17 @@
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" t="str">
-        <f t="shared" si="0"/>
-        <v>schelvispekel</v>
+        <f>LOWER(SUBSTITUTE(B33," ", "_"))</f>
+        <v>ketel1</v>
       </c>
       <c r="B33" t="s">
-        <v>30</v>
+        <v>53</v>
       </c>
       <c r="C33">
         <v>35</v>
       </c>
       <c r="D33" s="1">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="E33">
         <v>40</v>
@@ -1242,17 +1245,17 @@
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" t="str">
-        <f t="shared" si="0"/>
-        <v>cointreau</v>
+        <f>LOWER(SUBSTITUTE(B34," ", "_"))</f>
+        <v>kontiki</v>
       </c>
       <c r="B34" t="s">
-        <v>31</v>
+        <v>54</v>
       </c>
       <c r="C34">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="D34" s="1">
-        <v>2.2999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="E34">
         <v>40</v>
@@ -1260,17 +1263,17 @@
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" t="str">
-        <f t="shared" si="0"/>
-        <v>friesengeist</v>
+        <f>LOWER(SUBSTITUTE(B35," ", "_"))</f>
+        <v>kuyper_bessen</v>
       </c>
       <c r="B35" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="C35">
-        <v>56</v>
+        <v>20</v>
       </c>
       <c r="D35" s="1">
-        <v>2.2999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="E35">
         <v>40</v>
@@ -1278,17 +1281,17 @@
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" t="str">
-        <f t="shared" si="0"/>
-        <v>tanqueray_gin</v>
+        <f>LOWER(SUBSTITUTE(B36," ", "_"))</f>
+        <v>kuyper_blueberry</v>
       </c>
       <c r="B36" t="s">
-        <v>33</v>
+        <v>63</v>
       </c>
       <c r="C36">
-        <v>45.7</v>
+        <v>17</v>
       </c>
       <c r="D36" s="1">
-        <v>2.2999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="E36">
         <v>40</v>
@@ -1296,17 +1299,17 @@
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" t="str">
-        <f t="shared" si="0"/>
-        <v>grand_marnier</v>
+        <f>LOWER(SUBSTITUTE(B37," ", "_"))</f>
+        <v>kuyper_coconut</v>
       </c>
       <c r="B37" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="C37">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D37" s="1">
-        <v>2.2999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="E37">
         <v>40</v>
@@ -1314,17 +1317,17 @@
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" t="str">
-        <f t="shared" si="0"/>
-        <v>limoncello</v>
+        <f>LOWER(SUBSTITUTE(B38," ", "_"))</f>
+        <v>kuyper_marasquin</v>
       </c>
       <c r="B38" t="s">
-        <v>35</v>
+        <v>57</v>
       </c>
       <c r="C38">
-        <v>32</v>
+        <v>29</v>
       </c>
       <c r="D38" s="1">
-        <v>2.2999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="E38">
         <v>40</v>
@@ -1332,17 +1335,17 @@
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" t="str">
-        <f t="shared" si="0"/>
-        <v>tequila</v>
+        <f>LOWER(SUBSTITUTE(B39," ", "_"))</f>
+        <v>kuyper_pina_colada</v>
       </c>
       <c r="B39" t="s">
-        <v>36</v>
+        <v>59</v>
       </c>
       <c r="C39">
-        <v>38</v>
+        <v>15</v>
       </c>
       <c r="D39" s="1">
-        <v>2.2999999999999998</v>
+        <v>1.3</v>
       </c>
       <c r="E39">
         <v>40</v>
@@ -1350,17 +1353,17 @@
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" t="str">
-        <f t="shared" si="0"/>
-        <v>cognac</v>
+        <f>LOWER(SUBSTITUTE(B40," ", "_"))</f>
+        <v>licor_43</v>
       </c>
       <c r="B40" t="s">
-        <v>37</v>
+        <v>28</v>
       </c>
       <c r="C40">
-        <v>40</v>
+        <v>31</v>
       </c>
       <c r="D40" s="1">
-        <v>3</v>
+        <v>1.7</v>
       </c>
       <c r="E40">
         <v>40</v>
@@ -1368,17 +1371,17 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" t="str">
-        <f t="shared" si="0"/>
-        <v>stroh80</v>
+        <f>LOWER(SUBSTITUTE(B41," ", "_"))</f>
+        <v>limoncello</v>
       </c>
       <c r="B41" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="C41">
-        <v>80</v>
+        <v>32</v>
       </c>
       <c r="D41" s="1">
-        <v>3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E41">
         <v>40</v>
@@ -1386,17 +1389,17 @@
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" t="str">
-        <f t="shared" si="0"/>
-        <v>whiskey</v>
+        <f>LOWER(SUBSTITUTE(B42," ", "_"))</f>
+        <v>malibu</v>
       </c>
       <c r="B42" t="s">
-        <v>39</v>
+        <v>10</v>
       </c>
       <c r="C42">
-        <v>40</v>
+        <v>21</v>
       </c>
       <c r="D42" s="1">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="E42">
         <v>40</v>
@@ -1404,14 +1407,14 @@
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43" t="str">
-        <f t="shared" si="0"/>
-        <v>vodka</v>
+        <f>LOWER(SUBSTITUTE(B43," ", "_"))</f>
+        <v>martini</v>
       </c>
       <c r="B43" t="s">
-        <v>40</v>
+        <v>11</v>
       </c>
       <c r="C43">
-        <v>37.5</v>
+        <v>15</v>
       </c>
       <c r="D43" s="1">
         <v>1.3</v>
@@ -1422,14 +1425,14 @@
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44" t="str">
-        <f t="shared" si="0"/>
-        <v>sperma</v>
+        <f>LOWER(SUBSTITUTE(B44," ", "_"))</f>
+        <v>mede</v>
       </c>
       <c r="B44" t="s">
-        <v>41</v>
+        <v>12</v>
       </c>
       <c r="C44">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D44" s="1">
         <v>1.3</v>
@@ -1441,7 +1444,7 @@
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45" t="str">
-        <f t="shared" si="0"/>
+        <f>LOWER(SUBSTITUTE(B45," ", "_"))</f>
         <v>oranjebitter</v>
       </c>
       <c r="B45" t="s">
@@ -1460,14 +1463,14 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46" t="str">
-        <f t="shared" si="0"/>
-        <v>bols_apple_sour</v>
+        <f>LOWER(SUBSTITUTE(B46," ", "_"))</f>
+        <v>passao</v>
       </c>
       <c r="B46" t="s">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="C46">
-        <v>17</v>
+        <v>14.9</v>
       </c>
       <c r="D46" s="1">
         <v>1.3</v>
@@ -1479,17 +1482,17 @@
     </row>
     <row r="47" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A47" t="str">
-        <f t="shared" si="0"/>
-        <v>bacardi_black</v>
+        <f>LOWER(SUBSTITUTE(B47," ", "_"))</f>
+        <v>peach_tree</v>
       </c>
       <c r="B47" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="C47">
-        <v>38</v>
+        <v>20</v>
       </c>
       <c r="D47" s="1">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="E47">
         <v>40</v>
@@ -1498,17 +1501,17 @@
     </row>
     <row r="48" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A48" t="str">
-        <f t="shared" si="0"/>
-        <v>bacardi_blanca</v>
+        <f>LOWER(SUBSTITUTE(B48," ", "_"))</f>
+        <v>peerkorn</v>
       </c>
       <c r="B48" t="s">
-        <v>45</v>
+        <v>62</v>
       </c>
       <c r="C48">
-        <v>37.5</v>
+        <v>15</v>
       </c>
       <c r="D48" s="1">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="E48">
         <v>40</v>
@@ -1516,14 +1519,14 @@
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" t="str">
-        <f t="shared" si="0"/>
-        <v>bacardi_lemon</v>
+        <f>LOWER(SUBSTITUTE(B49," ", "_"))</f>
+        <v>pernod</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C49">
-        <v>32</v>
+        <v>40</v>
       </c>
       <c r="D49" s="1">
         <v>1.7</v>
@@ -1534,17 +1537,17 @@
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" t="str">
-        <f t="shared" si="0"/>
-        <v>bacardi_razz</v>
+        <f>LOWER(SUBSTITUTE(B50," ", "_"))</f>
+        <v>pisang_ambon</v>
       </c>
       <c r="B50" t="s">
-        <v>47</v>
+        <v>15</v>
       </c>
       <c r="C50">
-        <v>32</v>
+        <v>21</v>
       </c>
       <c r="D50" s="1">
-        <v>1.7</v>
+        <v>1.3</v>
       </c>
       <c r="E50">
         <v>40</v>
@@ -1552,14 +1555,14 @@
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" t="str">
-        <f t="shared" si="0"/>
-        <v>kuyper_blueberry</v>
+        <f>LOWER(SUBSTITUTE(B51," ", "_"))</f>
+        <v>puschkin_black</v>
       </c>
       <c r="B51" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
       <c r="C51">
-        <v>17</v>
+        <v>16.600000000000001</v>
       </c>
       <c r="D51" s="1">
         <v>1.3</v>
@@ -1570,14 +1573,14 @@
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" t="str">
-        <f t="shared" si="0"/>
-        <v>bols_blue_caracao</v>
+        <f>LOWER(SUBSTITUTE(B52," ", "_"))</f>
+        <v>safari</v>
       </c>
       <c r="B52" t="s">
-        <v>48</v>
+        <v>16</v>
       </c>
       <c r="C52">
-        <v>14.5</v>
+        <v>20</v>
       </c>
       <c r="D52" s="1">
         <v>1.3</v>
@@ -1588,17 +1591,17 @@
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" t="str">
-        <f t="shared" si="0"/>
-        <v>bols_crème_de_bananes</v>
+        <f>LOWER(SUBSTITUTE(B53," ", "_"))</f>
+        <v>sambuca</v>
       </c>
       <c r="B53" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="C53">
-        <v>15</v>
+        <v>38</v>
       </c>
       <c r="D53" s="1">
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
       <c r="E53">
         <v>40</v>
@@ -1606,17 +1609,17 @@
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" t="str">
-        <f t="shared" si="0"/>
-        <v>bols_crème_de_cassis</v>
+        <f>LOWER(SUBSTITUTE(B54," ", "_"))</f>
+        <v>schelvispekel</v>
       </c>
       <c r="B54" t="s">
-        <v>64</v>
+        <v>30</v>
       </c>
       <c r="C54">
-        <v>17</v>
+        <v>35</v>
       </c>
       <c r="D54" s="1">
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
       <c r="E54">
         <v>40</v>
@@ -1624,32 +1627,32 @@
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" t="str">
-        <f t="shared" si="0"/>
-        <v>estaminet</v>
+        <f>LOWER(SUBSTITUTE(B55," ", "_"))</f>
+        <v>sippers_bitter</v>
       </c>
       <c r="B55" t="s">
-        <v>50</v>
+        <v>17</v>
       </c>
       <c r="C55">
-        <v>5.2</v>
+        <v>30</v>
       </c>
       <c r="D55" s="1">
-        <v>1.2</v>
+        <v>1.3</v>
       </c>
       <c r="E55">
-        <v>250</v>
+        <v>40</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" t="str">
-        <f t="shared" si="0"/>
-        <v>hagel_en_donder</v>
+        <f>LOWER(SUBSTITUTE(B56," ", "_"))</f>
+        <v>sperma</v>
       </c>
       <c r="B56" t="s">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="C56">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D56" s="1">
         <v>1.3</v>
@@ -1660,35 +1663,35 @@
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" t="str">
-        <f t="shared" si="0"/>
-        <v>weihenstephaner</v>
+        <f>LOWER(SUBSTITUTE(B57," ", "_"))</f>
+        <v>stroh80</v>
       </c>
       <c r="B57" t="s">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="C57">
-        <v>5.4</v>
+        <v>80</v>
       </c>
       <c r="D57" s="1">
-        <v>1.7</v>
+        <v>3</v>
       </c>
       <c r="E57">
-        <v>300</v>
+        <v>40</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" t="str">
-        <f t="shared" si="0"/>
-        <v>kontiki</v>
+        <f>LOWER(SUBSTITUTE(B58," ", "_"))</f>
+        <v>tanqueray_gin</v>
       </c>
       <c r="B58" t="s">
-        <v>54</v>
+        <v>33</v>
       </c>
       <c r="C58">
-        <v>24</v>
+        <v>45.7</v>
       </c>
       <c r="D58" s="1">
-        <v>1.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E58">
         <v>40</v>
@@ -1696,17 +1699,17 @@
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" t="str">
-        <f t="shared" si="0"/>
-        <v>kuyper_bessen</v>
+        <f>LOWER(SUBSTITUTE(B59," ", "_"))</f>
+        <v>tequila</v>
       </c>
       <c r="B59" t="s">
-        <v>55</v>
+        <v>36</v>
       </c>
       <c r="C59">
-        <v>20</v>
+        <v>38</v>
       </c>
       <c r="D59" s="1">
-        <v>1.3</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E59">
         <v>40</v>
@@ -1714,14 +1717,14 @@
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" t="str">
-        <f t="shared" si="0"/>
-        <v>kuyper_coconut</v>
+        <f>LOWER(SUBSTITUTE(B60," ", "_"))</f>
+        <v>tia_maria</v>
       </c>
       <c r="B60" t="s">
-        <v>56</v>
+        <v>18</v>
       </c>
       <c r="C60">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D60" s="1">
         <v>1.3</v>
@@ -1732,14 +1735,14 @@
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" t="str">
-        <f t="shared" si="0"/>
-        <v>kuyper_marasquin</v>
+        <f>LOWER(SUBSTITUTE(B61," ", "_"))</f>
+        <v>vodka</v>
       </c>
       <c r="B61" t="s">
-        <v>57</v>
+        <v>40</v>
       </c>
       <c r="C61">
-        <v>29</v>
+        <v>37.5</v>
       </c>
       <c r="D61" s="1">
         <v>1.3</v>
@@ -1750,14 +1753,14 @@
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" t="str">
-        <f t="shared" si="0"/>
-        <v>kuyper_pina_colada</v>
+        <f>LOWER(SUBSTITUTE(B62," ", "_"))</f>
+        <v>vodka_rood</v>
       </c>
       <c r="B62" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="C62">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D62" s="1">
         <v>1.3</v>
@@ -1768,35 +1771,35 @@
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" t="str">
-        <f t="shared" si="0"/>
-        <v>puschkin_black</v>
+        <f>LOWER(SUBSTITUTE(B63," ", "_"))</f>
+        <v>weihenstephaner</v>
       </c>
       <c r="B63" t="s">
-        <v>60</v>
+        <v>52</v>
       </c>
       <c r="C63">
-        <v>16.600000000000001</v>
+        <v>5.4</v>
       </c>
       <c r="D63" s="1">
-        <v>1.3</v>
+        <v>1.7</v>
       </c>
       <c r="E63">
-        <v>40</v>
+        <v>300</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" t="str">
-        <f t="shared" si="0"/>
-        <v>vodka_rood</v>
+        <f>LOWER(SUBSTITUTE(B64," ", "_"))</f>
+        <v>whiskey</v>
       </c>
       <c r="B64" t="s">
-        <v>61</v>
+        <v>39</v>
       </c>
       <c r="C64">
-        <v>18</v>
+        <v>40</v>
       </c>
       <c r="D64" s="1">
-        <v>1.3</v>
+        <v>3</v>
       </c>
       <c r="E64">
         <v>40</v>

</xml_diff>